<commit_message>
Finally utilize Firebase to build the levels. Improve description in Level. Add helper function getLevels which calls on Firebase to populate levels in LevelBuilder. Call getLevels from GameViewController - is this the best way?
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94A2542-39EE-5949-AD4B-211390D9D077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3326BD5B-719D-9040-8DC7-50902D6C2031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10340" windowWidth="36000" windowHeight="11440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="levels" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="52">
   <si>
     <t>start</t>
   </si>
@@ -177,6 +177,21 @@
   </si>
   <si>
     <t>r5c5</t>
+  </si>
+  <si>
+    <t>gemOnIce</t>
+  </si>
+  <si>
+    <t>hammer</t>
+  </si>
+  <si>
+    <t>sword</t>
+  </si>
+  <si>
+    <t>enemy</t>
+  </si>
+  <si>
+    <t>warp</t>
   </si>
 </sst>
 </file>
@@ -319,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,6 +535,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,13 +705,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1046,16 +1068,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM9"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="15" width="10.83203125" style="6"/>
+    <col min="22" max="27" width="10.83203125" style="6"/>
+    <col min="34" max="39" width="10.83203125" style="6"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
@@ -1195,13 +1222,13 @@
       <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="J2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P2" t="s">
@@ -1220,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:B9" si="0">B2+1</f>
+        <f t="shared" ref="B3:B13" si="0">B2+1</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -1235,13 +1262,13 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="J3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P3" t="s">
@@ -1256,7 +1283,7 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A9" si="1">A3+1</f>
+        <f t="shared" ref="A4:A13" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4">
@@ -1275,13 +1302,13 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="J4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P4" t="s">
@@ -1315,13 +1342,13 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="J5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P5" t="s">
@@ -1355,13 +1382,13 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
-      <c r="J6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="J6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="P6" t="s">
@@ -1395,13 +1422,13 @@
       <c r="F7" t="s">
         <v>3</v>
       </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="J7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P7" t="s">
@@ -1435,13 +1462,13 @@
       <c r="F8" t="s">
         <v>1</v>
       </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="J8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="P8" t="s">
@@ -1478,16 +1505,16 @@
       <c r="G9" t="s">
         <v>3</v>
       </c>
-      <c r="J9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" t="s">
-        <v>3</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="J9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P9" t="s">
@@ -1502,17 +1529,360 @@
       <c r="S9" t="s">
         <v>1</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="W9" t="s">
-        <v>3</v>
-      </c>
-      <c r="X9" t="s">
+      <c r="W9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="X9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Y9" s="6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" t="s">
+        <v>47</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" t="s">
+        <v>7</v>
+      </c>
+      <c r="U10" t="s">
+        <v>7</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM10" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>50</v>
+      </c>
+      <c r="R11" t="s">
+        <v>51</v>
+      </c>
+      <c r="S11" t="s">
+        <v>3</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>47</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new level. Add fading game board when advancing levels.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3326BD5B-719D-9040-8DC7-50902D6C2031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6030BEB6-E367-BB42-BE5F-65175A6BDCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10340" windowWidth="36000" windowHeight="11440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="52">
   <si>
     <t>start</t>
   </si>
@@ -1068,13 +1068,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM13"/>
+  <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG13" sqref="AG13"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:B13" si="0">B2+1</f>
+        <f t="shared" ref="B3:B14" si="0">B2+1</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -1283,7 +1283,7 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A13" si="1">A3+1</f>
+        <f t="shared" ref="A4:A14" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4">
@@ -1491,55 +1491,34 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="P9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R9" t="s">
-        <v>5</v>
-      </c>
-      <c r="S9" t="s">
-        <v>1</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="X9" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.2">
@@ -1552,25 +1531,19 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>7</v>
@@ -1579,17 +1552,11 @@
         <v>7</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="P10" t="s">
         <v>7</v>
       </c>
@@ -1597,70 +1564,22 @@
         <v>7</v>
       </c>
       <c r="R10" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="S10" t="s">
         <v>1</v>
       </c>
-      <c r="T10" t="s">
-        <v>7</v>
-      </c>
-      <c r="U10" t="s">
-        <v>7</v>
-      </c>
       <c r="V10" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="W10" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X10" s="6" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="Y10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD10" t="s">
         <v>5</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM10" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.2">
@@ -1673,55 +1592,115 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>7</v>
+      </c>
+      <c r="R11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>7</v>
+      </c>
+      <c r="U11" t="s">
+        <v>7</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="AK11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q11" t="s">
-        <v>50</v>
-      </c>
-      <c r="R11" t="s">
-        <v>51</v>
-      </c>
-      <c r="S11" t="s">
-        <v>3</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>3</v>
+      <c r="AL11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM11" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
@@ -1734,7 +1713,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1743,25 +1722,46 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>7</v>
+        <v>48</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="P12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q12" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="R12" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="S12" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
@@ -1774,114 +1774,154 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
         <v>47</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>47</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" s="6" t="s">
+      <c r="J14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P13" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>1</v>
-      </c>
-      <c r="R13" t="s">
-        <v>1</v>
-      </c>
-      <c r="S13" t="s">
-        <v>1</v>
-      </c>
-      <c r="T13" t="s">
-        <v>1</v>
-      </c>
-      <c r="U13" t="s">
+      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
         <v>47</v>
       </c>
-      <c r="V13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="W13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="6" t="s">
+      <c r="V14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AB13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM13" s="6" t="s">
+      <c r="AB14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prevent continuing past lives = 0. Start to build out ContinueScene.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6030BEB6-E367-BB42-BE5F-65175A6BDCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63664BBC-7C6A-6447-AC34-4B0246E6C5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10340" windowWidth="36000" windowHeight="11440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="levels" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="52">
   <si>
     <t>start</t>
   </si>
@@ -1068,13 +1068,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM14"/>
+  <dimension ref="A1:AM18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1208,6 +1208,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
+        <f>A2</f>
         <v>0</v>
       </c>
       <c r="C2">
@@ -1247,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:B14" si="0">B2+1</f>
+        <f t="shared" ref="B3:B18" si="0">A3</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -1283,7 +1284,7 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A14" si="1">A3+1</f>
+        <f t="shared" ref="A4:A18" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4">
@@ -1451,16 +1452,16 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>1</v>
@@ -1469,13 +1470,13 @@
         <v>1</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="R8" t="s">
         <v>4</v>
@@ -1491,7 +1492,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -1500,16 +1501,16 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P9" t="s">
         <v>3</v>
@@ -1531,55 +1532,34 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
         <v>3</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="P10" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="Q10" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>5</v>
-      </c>
-      <c r="S10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="X10" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="Y10" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.2">
@@ -1592,115 +1572,34 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="R11" t="s">
-        <v>47</v>
-      </c>
-      <c r="S11" t="s">
-        <v>1</v>
-      </c>
-      <c r="T11" t="s">
-        <v>7</v>
-      </c>
-      <c r="U11" t="s">
-        <v>7</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ11" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="AK11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM11" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
@@ -1713,55 +1612,34 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="L12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" t="s">
         <v>4</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P12" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>50</v>
-      </c>
-      <c r="R12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S12" t="s">
-        <v>3</v>
-      </c>
-      <c r="V12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="W12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="X12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y12" s="6" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
@@ -1780,28 +1658,49 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>7</v>
+      </c>
+      <c r="R13" t="s">
+        <v>5</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="X13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="P13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" t="s">
-        <v>7</v>
+      <c r="Y13" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
@@ -1814,114 +1713,376 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="G14" t="s">
         <v>47</v>
       </c>
       <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I14" t="s">
+      <c r="M14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>7</v>
+      </c>
+      <c r="R14" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O14" s="6" t="s">
+      <c r="S14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
+        <v>7</v>
+      </c>
+      <c r="U14" t="s">
+        <v>7</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P14" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>1</v>
-      </c>
-      <c r="R14" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" t="s">
-        <v>1</v>
-      </c>
-      <c r="T14" t="s">
-        <v>1</v>
-      </c>
-      <c r="U14" t="s">
+      <c r="Y14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P15" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>50</v>
+      </c>
+      <c r="R15" t="s">
+        <v>51</v>
+      </c>
+      <c r="S15" t="s">
+        <v>3</v>
+      </c>
+      <c r="V15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>6</v>
+      </c>
+      <c r="R16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
         <v>47</v>
       </c>
-      <c r="V14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="W14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="6" t="s">
+      <c r="F17" t="s">
         <v>47</v>
       </c>
-      <c r="AB14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM14" s="6" t="s">
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" t="s">
+        <v>1</v>
+      </c>
+      <c r="T17" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>6</v>
+      </c>
+      <c r="R18" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hit twice if ice sliding into a dragon. Start working on shading launch based on time of day.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0F7A38-5686-6D4F-A972-B82F8ADEE7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44FDF79-1535-8144-BC75-AC39D87DE894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="52">
   <si>
     <t>start</t>
   </si>
@@ -59,139 +59,139 @@
     <t>marsh</t>
   </si>
   <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>moves</t>
+  </si>
+  <si>
+    <t>r0c0</t>
+  </si>
+  <si>
+    <t>r0c1</t>
+  </si>
+  <si>
+    <t>r0c2</t>
+  </si>
+  <si>
+    <t>r0c3</t>
+  </si>
+  <si>
+    <t>r0c4</t>
+  </si>
+  <si>
+    <t>r0c5</t>
+  </si>
+  <si>
+    <t>r1c0</t>
+  </si>
+  <si>
+    <t>r1c1</t>
+  </si>
+  <si>
+    <t>r1c2</t>
+  </si>
+  <si>
+    <t>r1c3</t>
+  </si>
+  <si>
+    <t>r1c4</t>
+  </si>
+  <si>
+    <t>r1c5</t>
+  </si>
+  <si>
+    <t>r2c0</t>
+  </si>
+  <si>
+    <t>r2c1</t>
+  </si>
+  <si>
+    <t>r2c2</t>
+  </si>
+  <si>
+    <t>r2c3</t>
+  </si>
+  <si>
+    <t>r2c4</t>
+  </si>
+  <si>
+    <t>r2c5</t>
+  </si>
+  <si>
+    <t>r3c0</t>
+  </si>
+  <si>
+    <t>r3c1</t>
+  </si>
+  <si>
+    <t>r3c2</t>
+  </si>
+  <si>
+    <t>r3c3</t>
+  </si>
+  <si>
+    <t>r3c4</t>
+  </si>
+  <si>
+    <t>r3c5</t>
+  </si>
+  <si>
+    <t>r4c0</t>
+  </si>
+  <si>
+    <t>r4c1</t>
+  </si>
+  <si>
+    <t>r4c2</t>
+  </si>
+  <si>
+    <t>r4c3</t>
+  </si>
+  <si>
+    <t>r4c4</t>
+  </si>
+  <si>
+    <t>r4c5</t>
+  </si>
+  <si>
+    <t>r5c0</t>
+  </si>
+  <si>
+    <t>r5c1</t>
+  </si>
+  <si>
+    <t>r5c2</t>
+  </si>
+  <si>
+    <t>r5c3</t>
+  </si>
+  <si>
+    <t>r5c4</t>
+  </si>
+  <si>
+    <t>r5c5</t>
+  </si>
+  <si>
+    <t>hammer</t>
+  </si>
+  <si>
+    <t>sword</t>
+  </si>
+  <si>
+    <t>enemy</t>
+  </si>
+  <si>
+    <t>warp</t>
+  </si>
+  <si>
+    <t>gemOnIce</t>
+  </si>
+  <si>
     <t>ice</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>moves</t>
-  </si>
-  <si>
-    <t>r0c0</t>
-  </si>
-  <si>
-    <t>r0c1</t>
-  </si>
-  <si>
-    <t>r0c2</t>
-  </si>
-  <si>
-    <t>r0c3</t>
-  </si>
-  <si>
-    <t>r0c4</t>
-  </si>
-  <si>
-    <t>r0c5</t>
-  </si>
-  <si>
-    <t>r1c0</t>
-  </si>
-  <si>
-    <t>r1c1</t>
-  </si>
-  <si>
-    <t>r1c2</t>
-  </si>
-  <si>
-    <t>r1c3</t>
-  </si>
-  <si>
-    <t>r1c4</t>
-  </si>
-  <si>
-    <t>r1c5</t>
-  </si>
-  <si>
-    <t>r2c0</t>
-  </si>
-  <si>
-    <t>r2c1</t>
-  </si>
-  <si>
-    <t>r2c2</t>
-  </si>
-  <si>
-    <t>r2c3</t>
-  </si>
-  <si>
-    <t>r2c4</t>
-  </si>
-  <si>
-    <t>r2c5</t>
-  </si>
-  <si>
-    <t>r3c0</t>
-  </si>
-  <si>
-    <t>r3c1</t>
-  </si>
-  <si>
-    <t>r3c2</t>
-  </si>
-  <si>
-    <t>r3c3</t>
-  </si>
-  <si>
-    <t>r3c4</t>
-  </si>
-  <si>
-    <t>r3c5</t>
-  </si>
-  <si>
-    <t>r4c0</t>
-  </si>
-  <si>
-    <t>r4c1</t>
-  </si>
-  <si>
-    <t>r4c2</t>
-  </si>
-  <si>
-    <t>r4c3</t>
-  </si>
-  <si>
-    <t>r4c4</t>
-  </si>
-  <si>
-    <t>r4c5</t>
-  </si>
-  <si>
-    <t>r5c0</t>
-  </si>
-  <si>
-    <t>r5c1</t>
-  </si>
-  <si>
-    <t>r5c2</t>
-  </si>
-  <si>
-    <t>r5c3</t>
-  </si>
-  <si>
-    <t>r5c4</t>
-  </si>
-  <si>
-    <t>r5c5</t>
-  </si>
-  <si>
-    <t>gemOnIce</t>
-  </si>
-  <si>
-    <t>hammer</t>
-  </si>
-  <si>
-    <t>sword</t>
-  </si>
-  <si>
-    <t>enemy</t>
-  </si>
-  <si>
-    <t>warp</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -713,6 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,13 +1069,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM18"/>
+  <dimension ref="A1:AM52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,121 +1087,121 @@
   <sheetData>
     <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
@@ -1284,7 +1285,7 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A18" si="1">A3+1</f>
+        <f t="shared" ref="A4:A52" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4">
@@ -1304,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>1</v>
@@ -1316,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R4" t="s">
         <v>4</v>
@@ -1344,7 +1345,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>1</v>
@@ -1356,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R5" t="s">
         <v>4</v>
@@ -1476,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R8" t="s">
         <v>4</v>
@@ -1553,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q10" t="s">
         <v>1</v>
@@ -1587,7 +1588,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>3</v>
@@ -1612,34 +1613,34 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
@@ -1652,55 +1653,34 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R13" t="s">
-        <v>5</v>
-      </c>
-      <c r="S13" t="s">
-        <v>1</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="X13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y13" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
@@ -1713,115 +1693,34 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
       </c>
-      <c r="G14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" t="s">
-        <v>7</v>
-      </c>
       <c r="J14" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q14" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="R14" t="s">
-        <v>47</v>
-      </c>
-      <c r="S14" t="s">
-        <v>1</v>
-      </c>
-      <c r="T14" t="s">
-        <v>7</v>
-      </c>
-      <c r="U14" t="s">
-        <v>7</v>
-      </c>
-      <c r="V14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="W14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM14" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.2">
@@ -1830,59 +1729,38 @@
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B15" si="2">A15</f>
         <v>13</v>
       </c>
       <c r="C15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q15" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="R15" t="s">
-        <v>51</v>
-      </c>
-      <c r="S15" t="s">
-        <v>3</v>
-      </c>
-      <c r="V15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="W15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="X15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y15" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.2">
@@ -1895,37 +1773,37 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="P16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1935,118 +1813,37 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" t="s">
         <v>47</v>
       </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="P17" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1</v>
-      </c>
       <c r="R17" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" t="s">
-        <v>1</v>
-      </c>
-      <c r="T17" t="s">
-        <v>1</v>
-      </c>
-      <c r="U17" t="s">
-        <v>47</v>
-      </c>
-      <c r="V17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="W17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM17" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2056,33 +1853,1416 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="P18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" ref="B19:B21" si="3">A19</f>
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>48</v>
+      </c>
+      <c r="R19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P20" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>48</v>
+      </c>
+      <c r="R20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>48</v>
+      </c>
+      <c r="R21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" ref="B22" si="4">A22</f>
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P22" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>48</v>
+      </c>
+      <c r="R22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" ref="B23:B26" si="5">A23</f>
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P24" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>50</v>
+      </c>
+      <c r="R24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P25" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>51</v>
+      </c>
+      <c r="R25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="4">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>49</v>
+      </c>
+      <c r="R26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="shared" ref="B27" si="6">A27</f>
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>47</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>50</v>
+      </c>
+      <c r="R27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" ref="B28:B42" si="7">A28</f>
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P28" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" si="7"/>
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P29" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>47</v>
+      </c>
+      <c r="R29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P30" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>50</v>
+      </c>
+      <c r="R30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="7"/>
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>6</v>
+      </c>
+      <c r="R31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>5</v>
+      </c>
+      <c r="R32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="7"/>
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P33" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>5</v>
+      </c>
+      <c r="R33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P34" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>5</v>
+      </c>
+      <c r="R34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="7"/>
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P35" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>5</v>
+      </c>
+      <c r="R35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="7"/>
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P36" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>47</v>
+      </c>
+      <c r="R36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="4">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P37" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>3</v>
+      </c>
+      <c r="R37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="4">
+        <f t="shared" si="7"/>
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P38" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>3</v>
+      </c>
+      <c r="R38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="4">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P39" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>6</v>
+      </c>
+      <c r="R39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B40" s="4">
+        <f t="shared" si="7"/>
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P40" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>47</v>
+      </c>
+      <c r="R40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B41" s="4">
+        <f t="shared" si="7"/>
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P41" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>49</v>
+      </c>
+      <c r="R41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B42" s="4">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" t="s">
+        <v>50</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P42" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>3</v>
+      </c>
+      <c r="R42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B43" s="4">
+        <f t="shared" ref="B43:B52" si="8">A43</f>
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" t="s">
+        <v>47</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P43" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>50</v>
+      </c>
+      <c r="R43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B44" s="4">
+        <f t="shared" si="8"/>
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P44" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>48</v>
+      </c>
+      <c r="R44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="4">
+        <f t="shared" si="8"/>
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P45" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>48</v>
+      </c>
+      <c r="R45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="4">
+        <f t="shared" si="8"/>
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" t="s">
+        <v>48</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P46" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>49</v>
+      </c>
+      <c r="R46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B47" s="4">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>50</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P47" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>48</v>
+      </c>
+      <c r="R47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B48" s="4">
+        <f t="shared" si="8"/>
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" t="s">
+        <v>5</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P48" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>48</v>
+      </c>
+      <c r="R48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B49" s="4">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" t="s">
+        <v>50</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P49" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>49</v>
+      </c>
+      <c r="R49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B50" s="4">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50" t="s">
+        <v>46</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P50" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>5</v>
+      </c>
+      <c r="R50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B51" s="4">
+        <f t="shared" si="8"/>
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" t="s">
+        <v>50</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>6</v>
+      </c>
+      <c r="R51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B52" s="4">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>3</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P52" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>5</v>
+      </c>
+      <c r="R52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T52" s="7"/>
+      <c r="U52" s="7"/>
+      <c r="V52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="X52" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y52" s="6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Redesign objects (gems, items, enemy, boulder, warp) so that it now overlays on top of terrain. Had to basically re-engineer everything. Refactor everywhere.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E285886-900E-324F-94FF-40E634FCBBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF3692A-F9A0-8340-AE3A-B9EDF578F3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="levels" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">levels!$A$1:$AM$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">levels!$A$1:$BW$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="86">
   <si>
     <t>start</t>
   </si>
@@ -44,9 +44,6 @@
     <t>grass</t>
   </si>
   <si>
-    <t>endOpen</t>
-  </si>
-  <si>
     <t>gem</t>
   </si>
   <si>
@@ -188,10 +185,115 @@
     <t>warp</t>
   </si>
   <si>
-    <t>gemOnIce</t>
-  </si>
-  <si>
     <t>ice</t>
+  </si>
+  <si>
+    <t>s0d0</t>
+  </si>
+  <si>
+    <t>s0d1</t>
+  </si>
+  <si>
+    <t>s0d2</t>
+  </si>
+  <si>
+    <t>s0d3</t>
+  </si>
+  <si>
+    <t>s0d4</t>
+  </si>
+  <si>
+    <t>s0d5</t>
+  </si>
+  <si>
+    <t>s1d0</t>
+  </si>
+  <si>
+    <t>s1d1</t>
+  </si>
+  <si>
+    <t>s1d2</t>
+  </si>
+  <si>
+    <t>s1d3</t>
+  </si>
+  <si>
+    <t>s1d4</t>
+  </si>
+  <si>
+    <t>s1d5</t>
+  </si>
+  <si>
+    <t>s2d0</t>
+  </si>
+  <si>
+    <t>s2d1</t>
+  </si>
+  <si>
+    <t>s2d2</t>
+  </si>
+  <si>
+    <t>s2d3</t>
+  </si>
+  <si>
+    <t>s2d4</t>
+  </si>
+  <si>
+    <t>s2d5</t>
+  </si>
+  <si>
+    <t>s3d0</t>
+  </si>
+  <si>
+    <t>s3d1</t>
+  </si>
+  <si>
+    <t>s3d2</t>
+  </si>
+  <si>
+    <t>s3d3</t>
+  </si>
+  <si>
+    <t>s3d4</t>
+  </si>
+  <si>
+    <t>s3d5</t>
+  </si>
+  <si>
+    <t>s4d0</t>
+  </si>
+  <si>
+    <t>s4d1</t>
+  </si>
+  <si>
+    <t>s4d2</t>
+  </si>
+  <si>
+    <t>s4d3</t>
+  </si>
+  <si>
+    <t>s4d4</t>
+  </si>
+  <si>
+    <t>s4d5</t>
+  </si>
+  <si>
+    <t>s5d0</t>
+  </si>
+  <si>
+    <t>s5d1</t>
+  </si>
+  <si>
+    <t>s5d2</t>
+  </si>
+  <si>
+    <t>s5d3</t>
+  </si>
+  <si>
+    <t>s5d4</t>
+  </si>
+  <si>
+    <t>s5d5</t>
   </si>
 </sst>
 </file>
@@ -334,7 +436,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,6 +646,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -705,7 +819,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -713,7 +827,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1069,143 +1185,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM61"/>
+  <dimension ref="A1:BW61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="BK3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I45" sqref="I45"/>
+      <selection pane="bottomRight" activeCell="BP17" sqref="BP17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="10" max="15" width="10.83203125" style="6"/>
-    <col min="16" max="21" width="10.83203125" style="7"/>
     <col min="22" max="27" width="10.83203125" style="6"/>
     <col min="34" max="39" width="10.83203125" style="6"/>
+    <col min="46" max="51" width="10.83203125" style="8"/>
+    <col min="58" max="63" width="10.83203125" style="8"/>
+    <col min="70" max="75" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AM1" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="BC1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BH1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="BI1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="BJ1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="BK1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="BM1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="BS1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="BT1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BV1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="BW1" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1234,17 +1460,17 @@
       <c r="L2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <f>A2+1</f>
         <v>1</v>
@@ -1263,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>1</v>
@@ -1274,17 +1500,20 @@
       <c r="L3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A61" si="1">A3+1</f>
         <v>2</v>
@@ -1303,10 +1532,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>1</v>
@@ -1314,17 +1543,23 @@
       <c r="L4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT4" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1343,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>1</v>
@@ -1354,17 +1589,23 @@
       <c r="L5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1383,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>1</v>
@@ -1392,19 +1633,28 @@
         <v>1</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1420,31 +1670,40 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="P7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU7" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1460,10 +1719,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>1</v>
@@ -1472,19 +1731,31 @@
         <v>1</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1500,10 +1771,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>1</v>
@@ -1514,17 +1785,23 @@
       <c r="L9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="P9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>5</v>
+      </c>
+      <c r="R9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1540,31 +1817,46 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="L10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1580,31 +1872,52 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R11" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1620,31 +1933,52 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1660,31 +1994,46 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1700,31 +2049,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1737,34 +2095,46 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1780,31 +2150,52 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R16" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1823,28 +2214,43 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1860,31 +2266,52 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="J18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP18" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="AT18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB18" t="s">
         <v>48</v>
       </c>
-      <c r="L18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P18" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1900,31 +2327,52 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1940,31 +2388,52 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO20" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" s="6" t="s">
+      <c r="AP20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ20" t="s">
         <v>48</v>
       </c>
-      <c r="L20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R20" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="BA20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1980,31 +2449,52 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ21" t="s">
         <v>46</v>
       </c>
-      <c r="F21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R21" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="BA21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -2020,31 +2510,46 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ22" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -2060,10 +2565,10 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>1</v>
@@ -2072,19 +2577,25 @@
         <v>1</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R23" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV23" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -2100,31 +2611,37 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="P24" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="P24" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>49</v>
+      </c>
+      <c r="R24" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -2140,31 +2657,40 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>1</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="R25" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="P25" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>49</v>
+      </c>
+      <c r="R25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV25" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -2186,25 +2712,34 @@
         <v>1</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="P26" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R26" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="P26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU26" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -2223,28 +2758,40 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="R27" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="P27" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>49</v>
+      </c>
+      <c r="R27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA27" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -2260,31 +2807,49 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R28" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -2306,25 +2871,37 @@
         <v>1</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="R29" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P29" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT29" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ29" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -2340,31 +2917,49 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P30" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q30" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="R30" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P30" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>49</v>
+      </c>
+      <c r="R30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -2380,31 +2975,43 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L31" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P31" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
         <v>5</v>
       </c>
-      <c r="P31" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R31" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R31" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU31" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV31" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -2420,31 +3027,43 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K32" s="6" t="s">
         <v>1</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="P32" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q32" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R32" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="P32" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT32" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ32" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA32" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -2457,34 +3076,55 @@
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q33" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R33" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ33" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -2500,31 +3140,52 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P34" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q34" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R34" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P34" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>1</v>
+      </c>
+      <c r="R34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU34" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV34" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ34" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -2540,31 +3201,52 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P35" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R35" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO35" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT35" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU35" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ35" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA35" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2577,34 +3259,55 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E36" t="s">
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="P36" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q36" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="R36" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>1</v>
+      </c>
+      <c r="R36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP36" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV36" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ36" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA36" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2620,31 +3323,52 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P37" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q37" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R37" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P37" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>1</v>
+      </c>
+      <c r="R37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO37" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP37" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU37" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA37" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2660,31 +3384,52 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="L38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P38" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>1</v>
+      </c>
+      <c r="R38" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO38" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP38" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU38" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="P38" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q38" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R38" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="AV38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA38" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2700,31 +3445,46 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K39" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P39" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q39" t="s">
         <v>5</v>
       </c>
-      <c r="L39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R39" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R39" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP39" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ39" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2740,31 +3500,46 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
         <v>5</v>
       </c>
-      <c r="F40" t="s">
-        <v>6</v>
-      </c>
       <c r="J40" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P40" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q40" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="R40" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="P40" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>1</v>
+      </c>
+      <c r="R40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO40" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV40" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA40" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2780,31 +3555,52 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P41" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q41" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P41" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>1</v>
+      </c>
+      <c r="R41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO41" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP41" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT41" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="AU41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ41" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA41" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2820,31 +3616,46 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q42" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R42" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>1</v>
+      </c>
+      <c r="R42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO42" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP42" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ42" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2860,31 +3671,52 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F43" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q43" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="R43" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="P43" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>49</v>
+      </c>
+      <c r="R43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT43" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU43" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV43" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ43" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2900,31 +3732,52 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P44" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q44" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R44" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P44" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>1</v>
+      </c>
+      <c r="R44" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT44" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU44" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ44" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="BA44" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2940,31 +3793,52 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P45" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q45" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R45" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P45" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>1</v>
+      </c>
+      <c r="R45" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO45" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP45" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU45" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ45" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA45" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2980,31 +3854,52 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F46" t="s">
+        <v>1</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P46" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>1</v>
+      </c>
+      <c r="R46" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO46" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP46" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J46" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P46" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q46" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R46" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="AV46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA46" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -3020,31 +3915,43 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P47" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q47" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R47" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="P47" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>1</v>
+      </c>
+      <c r="R47" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO47" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU47" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ47" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -3060,31 +3967,52 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P48" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q48" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P48" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>1</v>
+      </c>
+      <c r="R48" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO48" t="s">
         <v>48</v>
       </c>
-      <c r="R48" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AP48" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT48" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU48" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV48" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ48" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -3097,34 +4025,55 @@
         <v>8</v>
       </c>
       <c r="D49" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" t="s">
+        <v>49</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P49" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>1</v>
+      </c>
+      <c r="R49" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN49" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT49" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV49" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E49" t="s">
-        <v>50</v>
-      </c>
-      <c r="F49" t="s">
-        <v>50</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K49" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L49" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P49" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q49" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R49" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AZ49" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -3140,31 +4089,52 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F50" t="s">
+        <v>1</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P50" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO50" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP50" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT50" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU50" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV50" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ50" t="s">
         <v>46</v>
       </c>
-      <c r="J50" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L50" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P50" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q50" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R50" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="BA50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -3180,31 +4150,46 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L51" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P51" t="s">
         <v>5</v>
       </c>
-      <c r="P51" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q51" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R51" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Q51" t="s">
+        <v>5</v>
+      </c>
+      <c r="R51" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO51" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP51" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT51" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU51" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV51" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -3220,52 +4205,94 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P52" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q52" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R52" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="S52" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="P52" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>1</v>
+      </c>
+      <c r="R52" t="s">
+        <v>1</v>
+      </c>
+      <c r="S52" t="s">
+        <v>1</v>
       </c>
       <c r="V52" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W52" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X52" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="AO52" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP52" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ52" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT52" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU52" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV52" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW52" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ52" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA52" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB52" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC52" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF52" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG52" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH52" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -3281,52 +4308,94 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G53" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P53" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q53" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="R53" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="S53" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="P53" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>49</v>
+      </c>
+      <c r="R53" t="s">
+        <v>49</v>
+      </c>
+      <c r="S53" t="s">
+        <v>1</v>
       </c>
       <c r="V53" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="W53" s="6" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="X53" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Y53" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="AO53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ53" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV53" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ53" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA53" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB53" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC53" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF53" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG53" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH53" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -3342,52 +4411,94 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F54" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P54" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>1</v>
+      </c>
+      <c r="R54" t="s">
+        <v>1</v>
+      </c>
+      <c r="S54" t="s">
+        <v>1</v>
+      </c>
+      <c r="V54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO54" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP54" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ54" t="s">
         <v>48</v>
       </c>
-      <c r="G54" t="s">
-        <v>49</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K54" s="6" t="s">
+      <c r="AT54" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU54" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ54" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA54" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB54" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC54" t="s">
+        <v>48</v>
+      </c>
+      <c r="BF54" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L54" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M54" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P54" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q54" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R54" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="S54" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="V54" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="W54" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="X54" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y54" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="BG54" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH54" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -3400,55 +4511,97 @@
         <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P55" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>1</v>
+      </c>
+      <c r="R55" t="s">
+        <v>3</v>
+      </c>
+      <c r="S55" t="s">
+        <v>1</v>
+      </c>
+      <c r="V55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN55" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO55" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP55" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ55" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT55" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV55" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F55" t="s">
+      <c r="AW55" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ55" t="s">
         <v>46</v>
       </c>
-      <c r="G55" t="s">
-        <v>5</v>
-      </c>
-      <c r="J55" s="6" t="s">
+      <c r="BA55" t="s">
         <v>48</v>
       </c>
-      <c r="K55" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L55" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M55" s="6" t="s">
+      <c r="BC55" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF55" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG55" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="P55" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q55" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R55" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="S55" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="V55" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W55" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="X55" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y55" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="BH55" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI55" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -3464,52 +4617,94 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P56" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q56" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R56" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="S56" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="P56" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>1</v>
+      </c>
+      <c r="R56" t="s">
+        <v>1</v>
+      </c>
+      <c r="S56" t="s">
+        <v>1</v>
       </c>
       <c r="V56" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W56" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X56" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Y56" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="AO56" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP56" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ56" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT56" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ56" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA56" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB56" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC56" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH56" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -3525,52 +4720,82 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P57" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q57" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R57" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="S57" s="7" t="s">
-        <v>48</v>
+        <v>1</v>
+      </c>
+      <c r="P57" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>5</v>
+      </c>
+      <c r="R57" t="s">
+        <v>5</v>
+      </c>
+      <c r="S57" t="s">
+        <v>1</v>
       </c>
       <c r="V57" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="W57" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="X57" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="Y57" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="AO57" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP57" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT57" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW57" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ57" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC57" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF57" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BG57" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH57" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -3586,52 +4811,76 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P58" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q58" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R58" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="S58" s="7" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="P58" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>1</v>
+      </c>
+      <c r="R58" t="s">
+        <v>5</v>
+      </c>
+      <c r="S58" t="s">
+        <v>5</v>
       </c>
       <c r="V58" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X58" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y58" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="AP58" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ58" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV58" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW58" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ58" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA58" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF58" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG58" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -3647,52 +4896,91 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="L59" s="6" t="s">
         <v>1</v>
       </c>
       <c r="M59" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P59" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q59" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R59" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S59" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="P59" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>1</v>
+      </c>
+      <c r="R59" t="s">
+        <v>1</v>
+      </c>
+      <c r="S59" t="s">
+        <v>1</v>
       </c>
       <c r="V59" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W59" s="6" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="X59" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y59" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="AP59" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ59" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT59" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW59" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ59" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA59" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB59" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC59" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF59" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG59" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH59" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI59" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -3708,52 +4996,94 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G60" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K60" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P60" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>1</v>
+      </c>
+      <c r="R60" t="s">
+        <v>1</v>
+      </c>
+      <c r="S60" t="s">
+        <v>49</v>
+      </c>
+      <c r="V60" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W60" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X60" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y60" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO60" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP60" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ60" t="s">
         <v>48</v>
       </c>
-      <c r="L60" s="6" t="s">
+      <c r="AT60" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU60" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV60" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW60" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ60" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA60" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB60" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC60" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG60" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH60" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI60" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="M60" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P60" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q60" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R60" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S60" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="V60" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="W60" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X60" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y60" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -3775,47 +5105,65 @@
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L61" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M61" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P61" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q61" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="R61" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="S61" s="7" t="s">
+      <c r="P61" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>49</v>
+      </c>
+      <c r="R61" t="s">
+        <v>1</v>
+      </c>
+      <c r="S61" t="s">
         <v>1</v>
       </c>
       <c r="V61" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W61" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X61" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y61" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="AQ61" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV61" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB61" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF61" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG61" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI61" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:BW61" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Add gradient grass. Update sky to match new moon images.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF3692A-F9A0-8340-AE3A-B9EDF578F3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C9DE7-DD64-BC44-B290-E8F3F5BE9877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="86">
   <si>
     <t>start</t>
   </si>
@@ -819,7 +819,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -830,6 +830,7 @@
     <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1185,13 +1186,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BW61"/>
+  <dimension ref="A1:BW62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="BK3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AM36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BP17" sqref="BP17"/>
+      <selection pane="bottomRight" activeCell="AW73" sqref="AW73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1515,7 +1516,7 @@
     </row>
     <row r="4" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A61" si="1">A3+1</f>
+        <f t="shared" ref="A4:A62" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4">
@@ -5160,6 +5161,115 @@
       </c>
       <c r="BI61" s="8" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A62" s="4">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B62" s="4">
+        <f t="shared" ref="B62" si="10">A62</f>
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" t="s">
+        <v>5</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M62" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W62" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X62" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y62" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN62" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO62" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP62" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ62" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT62" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU62" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV62" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW62" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ62" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA62" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB62" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="BC62" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF62" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG62" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BH62" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BI62" s="8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hide status bar. Add new font: LuckiestBoy-Regular - so fitting! Move assets to Game Assets folder. Add dayMultiplier to have variable speeds for background and player animation in the LaunchScene. Move around ScoringEngine labels.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C9DE7-DD64-BC44-B290-E8F3F5BE9877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12592F6-D872-BA42-A427-089CE2B987F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="levels" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">levels!$A$1:$BW$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">levels!$A$1:$BX$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="88">
   <si>
     <t>start</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>s5d5</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Too hard for early on…</t>
   </si>
 </sst>
 </file>
@@ -819,7 +825,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -830,7 +836,6 @@
     <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1186,26 +1191,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BW62"/>
+  <dimension ref="A1:BX77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AM36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="BO7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AW73" sqref="AW73"/>
+      <selection pane="bottomRight" activeCell="BX13" sqref="BX13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="15" width="10.83203125" style="6"/>
-    <col min="22" max="27" width="10.83203125" style="6"/>
-    <col min="34" max="39" width="10.83203125" style="6"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="15" width="10.83203125" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="21" width="10.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="27" width="10.83203125" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="33" width="10.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="39" width="10.83203125" style="6" customWidth="1" outlineLevel="1"/>
     <col min="46" max="51" width="10.83203125" style="8"/>
     <col min="58" max="63" width="10.83203125" style="8"/>
     <col min="70" max="75" width="10.83203125" style="8"/>
+    <col min="76" max="76" width="82.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:76" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1431,8 +1441,11 @@
       <c r="BW1" s="9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.2">
+      <c r="BX1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1471,7 +1484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <f>A2+1</f>
         <v>1</v>
@@ -1514,9 +1527,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A62" si="1">A3+1</f>
+        <f t="shared" ref="A4:A67" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4">
@@ -1560,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1606,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1655,7 +1668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1704,7 +1717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1756,7 +1769,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1802,7 +1815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1857,7 +1870,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1918,7 +1931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1979,7 +1992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2033,8 +2046,11 @@
       <c r="BA13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.2">
+      <c r="BX13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2083,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2135,7 +2151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -5173,49 +5189,49 @@
         <v>60</v>
       </c>
       <c r="C62">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D62" t="s">
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="F62" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="G62" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>49</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="L62" s="6" t="s">
         <v>49</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P62" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q62" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R62" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S62" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P62" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>49</v>
+      </c>
+      <c r="R62" t="s">
+        <v>49</v>
+      </c>
+      <c r="S62" t="s">
         <v>1</v>
       </c>
       <c r="V62" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W62" s="6" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="X62" s="6" t="s">
         <v>1</v>
@@ -5223,57 +5239,1290 @@
       <c r="Y62" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AN62" t="s">
-        <v>2</v>
-      </c>
       <c r="AO62" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP62" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ62" t="s">
         <v>46</v>
       </c>
-      <c r="AP62" t="s">
-        <v>4</v>
-      </c>
-      <c r="AQ62" t="s">
-        <v>47</v>
-      </c>
       <c r="AT62" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AU62" s="8" t="s">
+      <c r="AV62" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ62" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA62" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB62" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC62" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF62" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH62" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A63" s="4">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B63" s="4">
+        <f t="shared" ref="B63:B75" si="11">A63</f>
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>49</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M63" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P63" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>1</v>
+      </c>
+      <c r="R63" t="s">
+        <v>1</v>
+      </c>
+      <c r="S63" t="s">
+        <v>49</v>
+      </c>
+      <c r="V63" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="X63" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y63" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP63" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ63" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW63" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC63" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF63" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BH63" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI63" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A64" s="4">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B64" s="4">
+        <f t="shared" si="11"/>
+        <v>62</v>
+      </c>
+      <c r="C64">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>1</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P64" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>1</v>
+      </c>
+      <c r="R64" t="s">
+        <v>1</v>
+      </c>
+      <c r="S64" t="s">
+        <v>1</v>
+      </c>
+      <c r="V64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y64" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT64" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AV62" s="8" t="s">
+      <c r="AU64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV64" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ64" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA64" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB64" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC64" t="s">
+        <v>48</v>
+      </c>
+      <c r="BF64" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AW62" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ62" s="10" t="s">
+      <c r="BH64" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A65" s="4">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B65" s="4">
+        <f t="shared" si="11"/>
+        <v>63</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>49</v>
+      </c>
+      <c r="F65" t="s">
+        <v>5</v>
+      </c>
+      <c r="G65" t="s">
+        <v>1</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L65" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P65" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>49</v>
+      </c>
+      <c r="R65" t="s">
+        <v>49</v>
+      </c>
+      <c r="S65" t="s">
+        <v>1</v>
+      </c>
+      <c r="V65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W65" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV65" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC65" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="B66" s="4">
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>16</v>
+      </c>
+      <c r="D66" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1</v>
+      </c>
+      <c r="G66" t="s">
+        <v>1</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P66" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>1</v>
+      </c>
+      <c r="R66" t="s">
+        <v>5</v>
+      </c>
+      <c r="S66" t="s">
+        <v>1</v>
+      </c>
+      <c r="V66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y66" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP66" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ66" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT66" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ66" t="s">
         <v>45</v>
       </c>
-      <c r="BA62" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB62" s="10" t="s">
+      <c r="BA66" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC66" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF66" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="BC62" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BF62" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="BG62" s="8" t="s">
+      <c r="BG66" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="B67" s="4">
+        <f t="shared" si="11"/>
+        <v>65</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" t="s">
+        <v>49</v>
+      </c>
+      <c r="G67" t="s">
+        <v>49</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P67" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>49</v>
+      </c>
+      <c r="R67" t="s">
+        <v>49</v>
+      </c>
+      <c r="S67" t="s">
+        <v>49</v>
+      </c>
+      <c r="V67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y67" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU67" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA67" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC67" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF67" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH67" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <f t="shared" ref="A68:A77" si="12">A67+1</f>
+        <v>66</v>
+      </c>
+      <c r="B68" s="4">
+        <f t="shared" si="11"/>
+        <v>66</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68" t="s">
+        <v>49</v>
+      </c>
+      <c r="G68" t="s">
+        <v>49</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P68" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>49</v>
+      </c>
+      <c r="R68" t="s">
+        <v>49</v>
+      </c>
+      <c r="S68" t="s">
+        <v>49</v>
+      </c>
+      <c r="V68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y68" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP68" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV68" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW68" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ68" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC68" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG68" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="BH62" s="8" t="s">
+    </row>
+    <row r="69" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <f t="shared" si="12"/>
+        <v>67</v>
+      </c>
+      <c r="B69" s="4">
+        <f t="shared" si="11"/>
+        <v>67</v>
+      </c>
+      <c r="C69">
+        <v>8</v>
+      </c>
+      <c r="D69" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F69" t="s">
+        <v>49</v>
+      </c>
+      <c r="G69" t="s">
+        <v>49</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P69" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>49</v>
+      </c>
+      <c r="R69" t="s">
+        <v>49</v>
+      </c>
+      <c r="S69" t="s">
+        <v>49</v>
+      </c>
+      <c r="V69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP69" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ69" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT69" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW69" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ69" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA69" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB69" t="s">
+        <v>45</v>
+      </c>
+      <c r="BG69" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A70" s="4">
+        <f t="shared" si="12"/>
+        <v>68</v>
+      </c>
+      <c r="B70" s="4">
+        <f t="shared" si="11"/>
+        <v>68</v>
+      </c>
+      <c r="C70">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" t="s">
+        <v>49</v>
+      </c>
+      <c r="G70" t="s">
+        <v>5</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L70" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P70" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>49</v>
+      </c>
+      <c r="R70" t="s">
+        <v>49</v>
+      </c>
+      <c r="S70" t="s">
+        <v>5</v>
+      </c>
+      <c r="V70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="X70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y70" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP70" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV70" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ70" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA70" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <f t="shared" si="12"/>
+        <v>69</v>
+      </c>
+      <c r="B71" s="4">
+        <f t="shared" si="11"/>
+        <v>69</v>
+      </c>
+      <c r="C71">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" t="s">
+        <v>49</v>
+      </c>
+      <c r="G71" t="s">
+        <v>49</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P71" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>49</v>
+      </c>
+      <c r="R71" t="s">
+        <v>49</v>
+      </c>
+      <c r="S71" t="s">
+        <v>49</v>
+      </c>
+      <c r="V71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y71" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ71" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW71" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ71" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA71" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB71" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF71" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="B72" s="4">
+        <f t="shared" si="11"/>
+        <v>70</v>
+      </c>
+      <c r="C72">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>49</v>
+      </c>
+      <c r="F72" t="s">
+        <v>49</v>
+      </c>
+      <c r="G72" t="s">
+        <v>49</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P72" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>49</v>
+      </c>
+      <c r="R72" t="s">
+        <v>49</v>
+      </c>
+      <c r="S72" t="s">
+        <v>49</v>
+      </c>
+      <c r="V72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y72" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ72" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT72" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV72" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW72" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ72" t="s">
+        <v>48</v>
+      </c>
+      <c r="BA72" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC72" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF72" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <f t="shared" si="12"/>
+        <v>71</v>
+      </c>
+      <c r="B73" s="4">
+        <f t="shared" si="11"/>
+        <v>71</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73" t="s">
+        <v>49</v>
+      </c>
+      <c r="G73" t="s">
+        <v>49</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P73" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>49</v>
+      </c>
+      <c r="R73" t="s">
+        <v>49</v>
+      </c>
+      <c r="S73" t="s">
+        <v>49</v>
+      </c>
+      <c r="V73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y73" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO73" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP73" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU73" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ73" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG73" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH73" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="BI62" s="8" t="s">
-        <v>2</v>
+    </row>
+    <row r="74" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <f t="shared" si="12"/>
+        <v>72</v>
+      </c>
+      <c r="B74" s="4">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>49</v>
+      </c>
+      <c r="F74" t="s">
+        <v>49</v>
+      </c>
+      <c r="G74" t="s">
+        <v>49</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P74" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>49</v>
+      </c>
+      <c r="R74" t="s">
+        <v>49</v>
+      </c>
+      <c r="S74" t="s">
+        <v>49</v>
+      </c>
+      <c r="V74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y74" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP74" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU74" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV74" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW74" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ74" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA74" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB74" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC74" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF74" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="BG74" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH74" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <f t="shared" si="12"/>
+        <v>73</v>
+      </c>
+      <c r="B75" s="4">
+        <f t="shared" si="11"/>
+        <v>73</v>
+      </c>
+      <c r="C75">
+        <v>9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>49</v>
+      </c>
+      <c r="F75" t="s">
+        <v>49</v>
+      </c>
+      <c r="G75" t="s">
+        <v>49</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P75" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>49</v>
+      </c>
+      <c r="R75" t="s">
+        <v>49</v>
+      </c>
+      <c r="S75" t="s">
+        <v>49</v>
+      </c>
+      <c r="V75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y75" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO75" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ75" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU75" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW75" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA75" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB75" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF75" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <f t="shared" si="12"/>
+        <v>74</v>
+      </c>
+      <c r="B76" s="4">
+        <f t="shared" ref="B76:B77" si="13">A76</f>
+        <v>74</v>
+      </c>
+      <c r="C76">
+        <v>7</v>
+      </c>
+      <c r="D76" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
+        <v>49</v>
+      </c>
+      <c r="G76" t="s">
+        <v>49</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P76" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>49</v>
+      </c>
+      <c r="R76" t="s">
+        <v>49</v>
+      </c>
+      <c r="S76" t="s">
+        <v>49</v>
+      </c>
+      <c r="V76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y76" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO76" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP76" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ76" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT76" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU76" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW76" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ76" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA76" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB76" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC76" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF76" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG76" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH76" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="B77" s="4">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="C77">
+        <v>11</v>
+      </c>
+      <c r="D77" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>49</v>
+      </c>
+      <c r="F77" t="s">
+        <v>49</v>
+      </c>
+      <c r="G77" t="s">
+        <v>49</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P77" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>49</v>
+      </c>
+      <c r="R77" t="s">
+        <v>49</v>
+      </c>
+      <c r="S77" t="s">
+        <v>49</v>
+      </c>
+      <c r="V77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y77" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ77" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU77" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV77" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG77" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH77" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BW61" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:BX77" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Score increments with animation.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12592F6-D872-BA42-A427-089CE2B987F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8651E2A-8527-DF42-8908-5007537D30EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="87">
   <si>
     <t>start</t>
   </si>
@@ -297,9 +297,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Too hard for early on…</t>
   </si>
 </sst>
 </file>
@@ -1194,10 +1191,10 @@
   <dimension ref="A1:BX77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="BO7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="BI4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BX13" sqref="BX13"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1490,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:B18" si="0">A3</f>
+        <f t="shared" ref="B3:B11" si="0">A3</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -1937,7 +1934,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B12:B21" si="2">A12</f>
         <v>10</v>
       </c>
       <c r="C12">
@@ -1998,11 +1995,11 @@
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -2011,43 +2008,34 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q13" t="s">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU13" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AV13" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AZ13" t="s">
         <v>2</v>
       </c>
       <c r="BA13" t="s">
-        <v>4</v>
-      </c>
-      <c r="BX13" t="s">
-        <v>87</v>
+        <v>2</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:76" x14ac:dyDescent="0.2">
@@ -2056,26 +2044,26 @@
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>1</v>
@@ -2087,15 +2075,18 @@
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT14" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="AV14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="BA14" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2105,32 +2096,32 @@
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" ref="B15" si="2">A15</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q15" t="s">
         <v>1</v>
@@ -2138,17 +2129,20 @@
       <c r="R15" t="s">
         <v>3</v>
       </c>
-      <c r="AO15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT15" s="8" t="s">
+      <c r="AP15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="AV15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ15" t="s">
         <v>2</v>
       </c>
       <c r="BA15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:76" x14ac:dyDescent="0.2">
@@ -2157,7 +2151,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C16">
@@ -2218,7 +2212,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C17">
@@ -2273,7 +2267,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C18">
@@ -2334,7 +2328,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4">
-        <f t="shared" ref="B19:B21" si="3">A19</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C19">
@@ -2395,7 +2389,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C20">
@@ -2456,7 +2450,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C21">
@@ -2517,7 +2511,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <f t="shared" ref="B22" si="4">A22</f>
+        <f t="shared" ref="B22" si="3">A22</f>
         <v>20</v>
       </c>
       <c r="C22">
@@ -2572,7 +2566,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4">
-        <f t="shared" ref="B23:B26" si="5">A23</f>
+        <f t="shared" ref="B23:B26" si="4">A23</f>
         <v>21</v>
       </c>
       <c r="C23">
@@ -2618,7 +2612,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="C24">
@@ -2664,7 +2658,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="C25">
@@ -2713,7 +2707,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="C26">
@@ -2762,7 +2756,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="4">
-        <f t="shared" ref="B27" si="6">A27</f>
+        <f t="shared" ref="B27" si="5">A27</f>
         <v>25</v>
       </c>
       <c r="C27">
@@ -2814,7 +2808,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="4">
-        <f t="shared" ref="B28:B42" si="7">A28</f>
+        <f t="shared" ref="B28:B42" si="6">A28</f>
         <v>26</v>
       </c>
       <c r="C28">
@@ -2872,7 +2866,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C29">
@@ -2924,7 +2918,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="C30">
@@ -2982,7 +2976,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="C31">
@@ -3034,7 +3028,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="C32">
@@ -3086,7 +3080,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="C33">
@@ -3147,7 +3141,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="C34">
@@ -3208,7 +3202,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
       <c r="C35">
@@ -3269,7 +3263,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="C36">
@@ -3330,7 +3324,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
       <c r="C37">
@@ -3391,7 +3385,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="C38">
@@ -3452,7 +3446,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="C39">
@@ -3507,7 +3501,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="C40">
@@ -3562,7 +3556,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="C41">
@@ -3623,7 +3617,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="C42">
@@ -3678,7 +3672,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="4">
-        <f t="shared" ref="B43:B52" si="8">A43</f>
+        <f t="shared" ref="B43:B52" si="7">A43</f>
         <v>41</v>
       </c>
       <c r="C43">
@@ -3739,7 +3733,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
       <c r="C44">
@@ -3800,7 +3794,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="C45">
@@ -3861,7 +3855,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="C46">
@@ -3922,7 +3916,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="C47">
@@ -3974,7 +3968,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
       <c r="C48">
@@ -4035,7 +4029,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>47</v>
       </c>
       <c r="C49">
@@ -4096,7 +4090,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="C50">
@@ -4157,7 +4151,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="C51">
@@ -4212,7 +4206,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="C52">
@@ -4315,7 +4309,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="4">
-        <f t="shared" ref="B53:B61" si="9">A53</f>
+        <f t="shared" ref="B53:B61" si="8">A53</f>
         <v>51</v>
       </c>
       <c r="C53">
@@ -4418,7 +4412,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>52</v>
       </c>
       <c r="C54">
@@ -4521,7 +4515,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>53</v>
       </c>
       <c r="C55">
@@ -4624,7 +4618,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>54</v>
       </c>
       <c r="C56">
@@ -4727,7 +4721,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="C57">
@@ -4818,7 +4812,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="C58">
@@ -4903,7 +4897,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="C59">
@@ -5003,7 +4997,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>58</v>
       </c>
       <c r="C60">
@@ -5106,7 +5100,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>59</v>
       </c>
       <c r="C61">
@@ -5185,7 +5179,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="4">
-        <f t="shared" ref="B62" si="10">A62</f>
+        <f t="shared" ref="B62" si="9">A62</f>
         <v>60</v>
       </c>
       <c r="C62">
@@ -5279,7 +5273,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="4">
-        <f t="shared" ref="B63:B75" si="11">A63</f>
+        <f t="shared" ref="B63:B75" si="10">A63</f>
         <v>61</v>
       </c>
       <c r="C63">
@@ -5361,7 +5355,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>62</v>
       </c>
       <c r="C64">
@@ -5452,7 +5446,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>63</v>
       </c>
       <c r="C65">
@@ -5519,7 +5513,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="C66">
@@ -5607,7 +5601,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>65</v>
       </c>
       <c r="C67">
@@ -5679,11 +5673,11 @@
     </row>
     <row r="68" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
-        <f t="shared" ref="A68:A77" si="12">A67+1</f>
+        <f t="shared" ref="A68:A77" si="11">A67+1</f>
         <v>66</v>
       </c>
       <c r="B68" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>66</v>
       </c>
       <c r="C68">
@@ -5758,13 +5752,13 @@
     </row>
     <row r="69" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
-        <f t="shared" si="12"/>
-        <v>67</v>
-      </c>
-      <c r="B69" s="4">
         <f t="shared" si="11"/>
         <v>67</v>
       </c>
+      <c r="B69" s="4">
+        <f t="shared" si="10"/>
+        <v>67</v>
+      </c>
       <c r="C69">
         <v>8</v>
       </c>
@@ -5843,13 +5837,13 @@
     </row>
     <row r="70" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
-        <f t="shared" si="12"/>
-        <v>68</v>
-      </c>
-      <c r="B70" s="4">
         <f t="shared" si="11"/>
         <v>68</v>
       </c>
+      <c r="B70" s="4">
+        <f t="shared" si="10"/>
+        <v>68</v>
+      </c>
       <c r="C70">
         <v>18</v>
       </c>
@@ -5919,13 +5913,13 @@
     </row>
     <row r="71" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
-        <f t="shared" si="12"/>
-        <v>69</v>
-      </c>
-      <c r="B71" s="4">
         <f t="shared" si="11"/>
         <v>69</v>
       </c>
+      <c r="B71" s="4">
+        <f t="shared" si="10"/>
+        <v>69</v>
+      </c>
       <c r="C71">
         <v>8</v>
       </c>
@@ -5998,13 +5992,13 @@
     </row>
     <row r="72" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
-        <f t="shared" si="12"/>
-        <v>70</v>
-      </c>
-      <c r="B72" s="4">
         <f t="shared" si="11"/>
         <v>70</v>
       </c>
+      <c r="B72" s="4">
+        <f t="shared" si="10"/>
+        <v>70</v>
+      </c>
       <c r="C72">
         <v>7</v>
       </c>
@@ -6083,13 +6077,13 @@
     </row>
     <row r="73" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
-        <f t="shared" si="12"/>
-        <v>71</v>
-      </c>
-      <c r="B73" s="4">
         <f t="shared" si="11"/>
         <v>71</v>
       </c>
+      <c r="B73" s="4">
+        <f t="shared" si="10"/>
+        <v>71</v>
+      </c>
       <c r="C73">
         <v>10</v>
       </c>
@@ -6171,13 +6165,13 @@
     </row>
     <row r="74" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
-        <f t="shared" si="12"/>
-        <v>72</v>
-      </c>
-      <c r="B74" s="4">
         <f t="shared" si="11"/>
         <v>72</v>
       </c>
+      <c r="B74" s="4">
+        <f t="shared" si="10"/>
+        <v>72</v>
+      </c>
       <c r="C74">
         <v>6</v>
       </c>
@@ -6265,13 +6259,13 @@
     </row>
     <row r="75" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
-        <f t="shared" si="12"/>
-        <v>73</v>
-      </c>
-      <c r="B75" s="4">
         <f t="shared" si="11"/>
         <v>73</v>
       </c>
+      <c r="B75" s="4">
+        <f t="shared" si="10"/>
+        <v>73</v>
+      </c>
       <c r="C75">
         <v>9</v>
       </c>
@@ -6347,11 +6341,11 @@
     </row>
     <row r="76" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>74</v>
       </c>
       <c r="B76" s="4">
-        <f t="shared" ref="B76:B77" si="13">A76</f>
+        <f t="shared" ref="B76:B77" si="12">A76</f>
         <v>74</v>
       </c>
       <c r="C76">
@@ -6447,11 +6441,11 @@
     </row>
     <row r="77" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="B77" s="4">
         <f t="shared" si="12"/>
-        <v>75</v>
-      </c>
-      <c r="B77" s="4">
-        <f t="shared" si="13"/>
         <v>75</v>
       </c>
       <c r="C77">

</xml_diff>

<commit_message>
Build out ChatSprite. Make GameboardSprite.spriteScale a static property.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8651E2A-8527-DF42-8908-5007537D30EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879B0B59-2365-5743-BA89-7159D2C72DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="levels" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">levels!$A$1:$BX$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">levels!$A$1:$BW$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="86">
   <si>
     <t>start</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>s5d5</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -1188,13 +1185,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BX77"/>
+  <dimension ref="A1:BW85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="BI4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="BP11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="BQ15" sqref="BQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1209,10 +1206,9 @@
     <col min="46" max="51" width="10.83203125" style="8"/>
     <col min="58" max="63" width="10.83203125" style="8"/>
     <col min="70" max="75" width="10.83203125" style="8"/>
-    <col min="76" max="76" width="82.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1438,11 +1434,8 @@
       <c r="BW1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="BX1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1481,7 +1474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <f>A2+1</f>
         <v>1</v>
@@ -1524,7 +1517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A67" si="1">A3+1</f>
         <v>2</v>
@@ -1570,7 +1563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1616,7 +1609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1665,7 +1658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1714,7 +1707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1766,7 +1759,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1812,7 +1805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1867,7 +1860,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1928,7 +1921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1989,7 +1982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2038,7 +2031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2090,7 +2083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2145,7 +2138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -5673,7 +5666,7 @@
     </row>
     <row r="68" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
-        <f t="shared" ref="A68:A77" si="11">A67+1</f>
+        <f t="shared" ref="A68:A85" si="11">A67+1</f>
         <v>66</v>
       </c>
       <c r="B68" s="4">
@@ -6515,8 +6508,688 @@
         <v>47</v>
       </c>
     </row>
+    <row r="78" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <f t="shared" si="11"/>
+        <v>76</v>
+      </c>
+      <c r="B78" s="4">
+        <f t="shared" ref="B78:B85" si="13">A78</f>
+        <v>76</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>49</v>
+      </c>
+      <c r="F78" t="s">
+        <v>49</v>
+      </c>
+      <c r="G78" t="s">
+        <v>49</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P78" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>49</v>
+      </c>
+      <c r="R78" t="s">
+        <v>49</v>
+      </c>
+      <c r="S78" t="s">
+        <v>49</v>
+      </c>
+      <c r="V78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y78" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO78" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP78" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ78" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW78" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ78" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB78" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC78" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF78" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <f t="shared" si="11"/>
+        <v>77</v>
+      </c>
+      <c r="B79" s="4">
+        <f t="shared" si="13"/>
+        <v>77</v>
+      </c>
+      <c r="C79">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" t="s">
+        <v>49</v>
+      </c>
+      <c r="G79" t="s">
+        <v>49</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P79" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>49</v>
+      </c>
+      <c r="R79" t="s">
+        <v>49</v>
+      </c>
+      <c r="S79" t="s">
+        <v>49</v>
+      </c>
+      <c r="V79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y79" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU79" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV79" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ79" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA79" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB79" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF79" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG79" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A80" s="4">
+        <f t="shared" si="11"/>
+        <v>78</v>
+      </c>
+      <c r="B80" s="4">
+        <f t="shared" si="13"/>
+        <v>78</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>49</v>
+      </c>
+      <c r="F80" t="s">
+        <v>49</v>
+      </c>
+      <c r="G80" t="s">
+        <v>49</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P80" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>49</v>
+      </c>
+      <c r="R80" t="s">
+        <v>49</v>
+      </c>
+      <c r="S80" t="s">
+        <v>49</v>
+      </c>
+      <c r="V80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y80" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO80" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP80" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ80" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB80" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC80" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF80" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH80" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <f t="shared" si="11"/>
+        <v>79</v>
+      </c>
+      <c r="B81" s="4">
+        <f t="shared" si="13"/>
+        <v>79</v>
+      </c>
+      <c r="C81">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>49</v>
+      </c>
+      <c r="F81" t="s">
+        <v>49</v>
+      </c>
+      <c r="G81" t="s">
+        <v>49</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P81" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>49</v>
+      </c>
+      <c r="R81" t="s">
+        <v>49</v>
+      </c>
+      <c r="S81" t="s">
+        <v>49</v>
+      </c>
+      <c r="V81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y81" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ81" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV81" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW81" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ81" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA81" t="s">
+        <v>45</v>
+      </c>
+      <c r="BC81" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF81" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG81" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH81" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <f t="shared" si="11"/>
+        <v>80</v>
+      </c>
+      <c r="B82" s="4">
+        <f t="shared" si="13"/>
+        <v>80</v>
+      </c>
+      <c r="C82">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>49</v>
+      </c>
+      <c r="F82" t="s">
+        <v>49</v>
+      </c>
+      <c r="G82" t="s">
+        <v>49</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P82" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>49</v>
+      </c>
+      <c r="R82" t="s">
+        <v>49</v>
+      </c>
+      <c r="S82" t="s">
+        <v>49</v>
+      </c>
+      <c r="V82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y82" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP82" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ82" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT82" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV82" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW82" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ82" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB82" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC82" t="s">
+        <v>48</v>
+      </c>
+      <c r="BF82" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG82" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH82" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <f t="shared" si="11"/>
+        <v>81</v>
+      </c>
+      <c r="B83" s="4">
+        <f t="shared" si="13"/>
+        <v>81</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>49</v>
+      </c>
+      <c r="F83" t="s">
+        <v>49</v>
+      </c>
+      <c r="G83" t="s">
+        <v>49</v>
+      </c>
+      <c r="J83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P83" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>49</v>
+      </c>
+      <c r="R83" t="s">
+        <v>49</v>
+      </c>
+      <c r="S83" t="s">
+        <v>49</v>
+      </c>
+      <c r="V83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y83" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT83" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU83" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV83" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ83" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB83" t="s">
+        <v>48</v>
+      </c>
+      <c r="BC83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <f t="shared" si="11"/>
+        <v>82</v>
+      </c>
+      <c r="B84" s="4">
+        <f t="shared" si="13"/>
+        <v>82</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>49</v>
+      </c>
+      <c r="F84" t="s">
+        <v>49</v>
+      </c>
+      <c r="G84" t="s">
+        <v>49</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P84" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>49</v>
+      </c>
+      <c r="R84" t="s">
+        <v>49</v>
+      </c>
+      <c r="S84" t="s">
+        <v>49</v>
+      </c>
+      <c r="V84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y84" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ84" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ84" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA84" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC84" t="s">
+        <v>45</v>
+      </c>
+      <c r="BF84" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH84" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <f t="shared" si="11"/>
+        <v>83</v>
+      </c>
+      <c r="B85" s="4">
+        <f t="shared" si="13"/>
+        <v>83</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+      <c r="D85" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1</v>
+      </c>
+      <c r="G85" t="s">
+        <v>1</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L85" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M85" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P85" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>49</v>
+      </c>
+      <c r="R85" t="s">
+        <v>49</v>
+      </c>
+      <c r="S85" t="s">
+        <v>1</v>
+      </c>
+      <c r="V85" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W85" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X85" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y85" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ85" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU85" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV85" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW85" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA85" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB85" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC85" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF85" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG85" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH85" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:BX77" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:BW77" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Change up the gameplay... dragon hits now affect health, not moves. Adjust levels w/ dragons, i.e. moveCount and healthCount.
</commit_message>
<xml_diff>
--- a/JSON/Levels.xlsx
+++ b/JSON/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879B0B59-2365-5743-BA89-7159D2C72DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86BA359-9E7F-3243-9255-EE196E667BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="3160" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="levels" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="86">
   <si>
     <t>start</t>
   </si>
@@ -1185,13 +1185,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BW85"/>
+  <dimension ref="A1:BW103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="BP11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="BJ64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BQ15" sqref="BQ15"/>
+      <selection pane="bottomRight" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:B11" si="0">A3</f>
+        <f>A3</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -1519,11 +1519,11 @@
     </row>
     <row r="4" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A67" si="1">A3+1</f>
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B4:B67" si="1">A4</f>
         <v>2</v>
       </c>
       <c r="C4">
@@ -1565,11 +1565,11 @@
     </row>
     <row r="5" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C5">
@@ -1611,11 +1611,11 @@
     </row>
     <row r="6" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C6">
@@ -1660,11 +1660,11 @@
     </row>
     <row r="7" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C7">
@@ -1709,13 +1709,13 @@
     </row>
     <row r="8" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
       <c r="C8">
         <v>8</v>
       </c>
@@ -1761,13 +1761,13 @@
     </row>
     <row r="9" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="C9">
         <v>8</v>
       </c>
@@ -1807,13 +1807,13 @@
     </row>
     <row r="10" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="C10">
         <v>7</v>
       </c>
@@ -1862,13 +1862,13 @@
     </row>
     <row r="11" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
       <c r="C11">
         <v>7</v>
       </c>
@@ -1923,13 +1923,13 @@
     </row>
     <row r="12" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="4">
-        <f t="shared" ref="B12:B21" si="2">A12</f>
-        <v>10</v>
-      </c>
       <c r="C12">
         <v>6</v>
       </c>
@@ -1984,13 +1984,13 @@
     </row>
     <row r="13" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="4">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
       <c r="C13">
         <v>7</v>
       </c>
@@ -2033,13 +2033,13 @@
     </row>
     <row r="14" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="4">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
       <c r="C14">
         <v>8</v>
       </c>
@@ -2085,13 +2085,13 @@
     </row>
     <row r="15" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="4">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
       <c r="C15">
         <v>10</v>
       </c>
@@ -2140,13 +2140,13 @@
     </row>
     <row r="16" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="4">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
       <c r="C16">
         <v>4</v>
       </c>
@@ -2201,13 +2201,13 @@
     </row>
     <row r="17" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="4">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
       <c r="C17">
         <v>8</v>
       </c>
@@ -2256,13 +2256,13 @@
     </row>
     <row r="18" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
       <c r="C18">
         <v>8</v>
       </c>
@@ -2317,13 +2317,13 @@
     </row>
     <row r="19" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="4">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
       <c r="C19">
         <v>6</v>
       </c>
@@ -2378,13 +2378,13 @@
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="4">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
       <c r="C20">
         <v>5</v>
       </c>
@@ -2439,13 +2439,13 @@
     </row>
     <row r="21" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="4">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="4">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
       <c r="C21">
         <v>6</v>
       </c>
@@ -2500,13 +2500,13 @@
     </row>
     <row r="22" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="4">
-        <f t="shared" ref="B22" si="3">A22</f>
-        <v>20</v>
-      </c>
       <c r="C22">
         <v>10</v>
       </c>
@@ -2555,13 +2555,13 @@
     </row>
     <row r="23" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="4">
-        <f t="shared" ref="B23:B26" si="4">A23</f>
-        <v>21</v>
-      </c>
       <c r="C23">
         <v>2</v>
       </c>
@@ -2601,13 +2601,13 @@
     </row>
     <row r="24" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="4">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
       <c r="C24">
         <v>3</v>
       </c>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="25" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="4">
-        <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
       <c r="C25">
         <v>4</v>
       </c>
@@ -2696,13 +2696,13 @@
     </row>
     <row r="26" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="4">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B26" s="4">
-        <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
       <c r="C26">
         <v>4</v>
       </c>
@@ -2745,13 +2745,13 @@
     </row>
     <row r="27" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="4">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="4">
-        <f t="shared" ref="B27" si="5">A27</f>
-        <v>25</v>
-      </c>
       <c r="C27">
         <v>7</v>
       </c>
@@ -2797,13 +2797,13 @@
     </row>
     <row r="28" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="4">
-        <f t="shared" ref="B28:B42" si="6">A28</f>
-        <v>26</v>
-      </c>
       <c r="C28">
         <v>5</v>
       </c>
@@ -2855,13 +2855,13 @@
     </row>
     <row r="29" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="4">
-        <f t="shared" si="6"/>
-        <v>27</v>
-      </c>
       <c r="C29">
         <v>7</v>
       </c>
@@ -2907,13 +2907,13 @@
     </row>
     <row r="30" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="4">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="4">
-        <f t="shared" si="6"/>
-        <v>28</v>
-      </c>
       <c r="C30">
         <v>6</v>
       </c>
@@ -2965,13 +2965,13 @@
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="4">
-        <f t="shared" si="6"/>
-        <v>29</v>
-      </c>
       <c r="C31">
         <v>7</v>
       </c>
@@ -3017,13 +3017,13 @@
     </row>
     <row r="32" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="4">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
       <c r="C32">
         <v>6</v>
       </c>
@@ -3069,13 +3069,13 @@
     </row>
     <row r="33" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="4">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B33" s="4">
-        <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
       <c r="C33">
         <v>8</v>
       </c>
@@ -3130,13 +3130,13 @@
     </row>
     <row r="34" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="4">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B34" s="4">
-        <f t="shared" si="6"/>
-        <v>32</v>
-      </c>
       <c r="C34">
         <v>8</v>
       </c>
@@ -3191,13 +3191,13 @@
     </row>
     <row r="35" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="4">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B35" s="4">
-        <f t="shared" si="6"/>
-        <v>33</v>
-      </c>
       <c r="C35">
         <v>6</v>
       </c>
@@ -3252,13 +3252,13 @@
     </row>
     <row r="36" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="4">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B36" s="4">
-        <f t="shared" si="6"/>
-        <v>34</v>
-      </c>
       <c r="C36">
         <v>7</v>
       </c>
@@ -3313,13 +3313,13 @@
     </row>
     <row r="37" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="4">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B37" s="4">
-        <f t="shared" si="6"/>
-        <v>35</v>
-      </c>
       <c r="C37">
         <v>6</v>
       </c>
@@ -3374,13 +3374,13 @@
     </row>
     <row r="38" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="4">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B38" s="4">
-        <f t="shared" si="6"/>
-        <v>36</v>
-      </c>
       <c r="C38">
         <v>6</v>
       </c>
@@ -3435,13 +3435,13 @@
     </row>
     <row r="39" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="4">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B39" s="4">
-        <f t="shared" si="6"/>
-        <v>37</v>
-      </c>
       <c r="C39">
         <v>11</v>
       </c>
@@ -3490,13 +3490,13 @@
     </row>
     <row r="40" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B40" s="4">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B40" s="4">
-        <f t="shared" si="6"/>
-        <v>38</v>
-      </c>
       <c r="C40">
         <v>10</v>
       </c>
@@ -3545,13 +3545,13 @@
     </row>
     <row r="41" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B41" s="4">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B41" s="4">
-        <f t="shared" si="6"/>
-        <v>39</v>
-      </c>
       <c r="C41">
         <v>7</v>
       </c>
@@ -3606,13 +3606,13 @@
     </row>
     <row r="42" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B42" s="4">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B42" s="4">
-        <f t="shared" si="6"/>
-        <v>40</v>
-      </c>
       <c r="C42">
         <v>7</v>
       </c>
@@ -3661,13 +3661,13 @@
     </row>
     <row r="43" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B43" s="4">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B43" s="4">
-        <f t="shared" ref="B43:B52" si="7">A43</f>
-        <v>41</v>
-      </c>
       <c r="C43">
         <v>9</v>
       </c>
@@ -3722,13 +3722,13 @@
     </row>
     <row r="44" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" s="4">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B44" s="4">
-        <f t="shared" si="7"/>
-        <v>42</v>
-      </c>
       <c r="C44">
         <v>7</v>
       </c>
@@ -3783,13 +3783,13 @@
     </row>
     <row r="45" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="4">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B45" s="4">
-        <f t="shared" si="7"/>
-        <v>43</v>
-      </c>
       <c r="C45">
         <v>9</v>
       </c>
@@ -3844,13 +3844,13 @@
     </row>
     <row r="46" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="4">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B46" s="4">
-        <f t="shared" si="7"/>
-        <v>44</v>
-      </c>
       <c r="C46">
         <v>8</v>
       </c>
@@ -3905,13 +3905,13 @@
     </row>
     <row r="47" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B47" s="4">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B47" s="4">
-        <f t="shared" si="7"/>
-        <v>45</v>
-      </c>
       <c r="C47">
         <v>7</v>
       </c>
@@ -3957,13 +3957,13 @@
     </row>
     <row r="48" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B48" s="4">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B48" s="4">
-        <f t="shared" si="7"/>
-        <v>46</v>
-      </c>
       <c r="C48">
         <v>6</v>
       </c>
@@ -4018,11 +4018,11 @@
     </row>
     <row r="49" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B49" s="4">
         <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="B49" s="4">
-        <f t="shared" si="7"/>
         <v>47</v>
       </c>
       <c r="C49">
@@ -4079,13 +4079,13 @@
     </row>
     <row r="50" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B50" s="4">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B50" s="4">
-        <f t="shared" si="7"/>
-        <v>48</v>
-      </c>
       <c r="C50">
         <v>6</v>
       </c>
@@ -4140,11 +4140,11 @@
     </row>
     <row r="51" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B51" s="4">
         <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="B51" s="4">
-        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="C51">
@@ -4195,13 +4195,13 @@
     </row>
     <row r="52" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B52" s="4">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B52" s="4">
-        <f t="shared" si="7"/>
-        <v>50</v>
-      </c>
       <c r="C52">
         <v>14</v>
       </c>
@@ -4298,13 +4298,13 @@
     </row>
     <row r="53" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B53" s="4">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B53" s="4">
-        <f t="shared" ref="B53:B61" si="8">A53</f>
-        <v>51</v>
-      </c>
       <c r="C53">
         <v>7</v>
       </c>
@@ -4401,13 +4401,13 @@
     </row>
     <row r="54" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B54" s="4">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B54" s="4">
-        <f t="shared" si="8"/>
-        <v>52</v>
-      </c>
       <c r="C54">
         <v>12</v>
       </c>
@@ -4504,13 +4504,13 @@
     </row>
     <row r="55" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B55" s="4">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B55" s="4">
-        <f t="shared" si="8"/>
-        <v>53</v>
-      </c>
       <c r="C55">
         <v>12</v>
       </c>
@@ -4607,13 +4607,13 @@
     </row>
     <row r="56" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B56" s="4">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B56" s="4">
-        <f t="shared" si="8"/>
-        <v>54</v>
-      </c>
       <c r="C56">
         <v>10</v>
       </c>
@@ -4710,13 +4710,13 @@
     </row>
     <row r="57" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B57" s="4">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B57" s="4">
-        <f t="shared" si="8"/>
-        <v>55</v>
-      </c>
       <c r="C57">
         <v>12</v>
       </c>
@@ -4801,13 +4801,13 @@
     </row>
     <row r="58" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B58" s="4">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B58" s="4">
-        <f t="shared" si="8"/>
-        <v>56</v>
-      </c>
       <c r="C58">
         <v>15</v>
       </c>
@@ -4886,13 +4886,13 @@
     </row>
     <row r="59" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B59" s="4">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B59" s="4">
-        <f t="shared" si="8"/>
-        <v>57</v>
-      </c>
       <c r="C59">
         <v>17</v>
       </c>
@@ -4986,13 +4986,13 @@
     </row>
     <row r="60" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B60" s="4">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B60" s="4">
-        <f t="shared" si="8"/>
-        <v>58</v>
-      </c>
       <c r="C60">
         <v>5</v>
       </c>
@@ -5089,13 +5089,13 @@
     </row>
     <row r="61" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B61" s="4">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B61" s="4">
-        <f t="shared" si="8"/>
-        <v>59</v>
-      </c>
       <c r="C61">
         <v>9</v>
       </c>
@@ -5168,13 +5168,13 @@
     </row>
     <row r="62" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B62" s="4">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B62" s="4">
-        <f t="shared" ref="B62" si="9">A62</f>
-        <v>60</v>
-      </c>
       <c r="C62">
         <v>14</v>
       </c>
@@ -5262,13 +5262,13 @@
     </row>
     <row r="63" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B63" s="4">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B63" s="4">
-        <f t="shared" ref="B63:B75" si="10">A63</f>
-        <v>61</v>
-      </c>
       <c r="C63">
         <v>12</v>
       </c>
@@ -5344,13 +5344,13 @@
     </row>
     <row r="64" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B64" s="4">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B64" s="4">
-        <f t="shared" si="10"/>
-        <v>62</v>
-      </c>
       <c r="C64">
         <v>12</v>
       </c>
@@ -5435,13 +5435,13 @@
     </row>
     <row r="65" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B65" s="4">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B65" s="4">
-        <f t="shared" si="10"/>
-        <v>63</v>
-      </c>
       <c r="C65">
         <v>6</v>
       </c>
@@ -5502,13 +5502,13 @@
     </row>
     <row r="66" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B66" s="4">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B66" s="4">
-        <f t="shared" si="10"/>
-        <v>64</v>
-      </c>
       <c r="C66">
         <v>16</v>
       </c>
@@ -5590,13 +5590,13 @@
     </row>
     <row r="67" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B67" s="4">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B67" s="4">
-        <f t="shared" si="10"/>
-        <v>65</v>
-      </c>
       <c r="C67">
         <v>7</v>
       </c>
@@ -5666,11 +5666,11 @@
     </row>
     <row r="68" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
-        <f t="shared" ref="A68:A85" si="11">A67+1</f>
+        <f t="shared" ref="A68:A103" si="2">A67+1</f>
         <v>66</v>
       </c>
       <c r="B68" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="B68:B103" si="3">A68</f>
         <v>66</v>
       </c>
       <c r="C68">
@@ -5745,11 +5745,11 @@
     </row>
     <row r="69" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="B69" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="C69">
@@ -5830,11 +5830,11 @@
     </row>
     <row r="70" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B70" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="C70">
@@ -5906,11 +5906,11 @@
     </row>
     <row r="71" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="B71" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
       <c r="C71">
@@ -5985,11 +5985,11 @@
     </row>
     <row r="72" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B72" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="C72">
@@ -6070,11 +6070,11 @@
     </row>
     <row r="73" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="B73" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C73">
@@ -6158,11 +6158,11 @@
     </row>
     <row r="74" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="B74" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="C74">
@@ -6252,11 +6252,11 @@
     </row>
     <row r="75" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="B75" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
       <c r="C75">
@@ -6334,11 +6334,11 @@
     </row>
     <row r="76" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="B76" s="4">
-        <f t="shared" ref="B76:B77" si="12">A76</f>
+        <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="C76">
@@ -6434,11 +6434,11 @@
     </row>
     <row r="77" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="B77" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="C77">
@@ -6510,11 +6510,11 @@
     </row>
     <row r="78" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="B78" s="4">
-        <f t="shared" ref="B78:B85" si="13">A78</f>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="C78">
@@ -6595,11 +6595,11 @@
     </row>
     <row r="79" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="B79" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="C79">
@@ -6677,11 +6677,11 @@
     </row>
     <row r="80" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="B80" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="C80">
@@ -6757,13 +6757,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="B81" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="C81">
@@ -6845,13 +6845,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B82" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C82">
@@ -6939,13 +6939,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="B83" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="C83">
@@ -7018,13 +7018,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="B84" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="C84">
@@ -7097,13 +7097,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="B85" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
       <c r="C85">
@@ -7186,6 +7186,1635 @@
       </c>
       <c r="BH85" s="8" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="B86" s="4">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>49</v>
+      </c>
+      <c r="F86" t="s">
+        <v>49</v>
+      </c>
+      <c r="G86" t="s">
+        <v>49</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L86" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M86" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P86" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>49</v>
+      </c>
+      <c r="R86" t="s">
+        <v>49</v>
+      </c>
+      <c r="S86" t="s">
+        <v>49</v>
+      </c>
+      <c r="V86" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W86" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X86" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y86" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO86" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP86" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ86" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU86" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV86" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW86" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA86" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB86" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC86" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI86" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="B87" s="4">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="C87">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3</v>
+      </c>
+      <c r="G87" t="s">
+        <v>1</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L87" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P87" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>49</v>
+      </c>
+      <c r="R87" t="s">
+        <v>49</v>
+      </c>
+      <c r="S87" t="s">
+        <v>1</v>
+      </c>
+      <c r="V87" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W87" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X87" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y87" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO87" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT87" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF87" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BG87" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH87" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="B88" s="4">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="C88">
+        <v>12</v>
+      </c>
+      <c r="D88" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>3</v>
+      </c>
+      <c r="F88" t="s">
+        <v>49</v>
+      </c>
+      <c r="G88" t="s">
+        <v>49</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L88" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P88" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>5</v>
+      </c>
+      <c r="R88" t="s">
+        <v>49</v>
+      </c>
+      <c r="S88" t="s">
+        <v>49</v>
+      </c>
+      <c r="V88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="X88" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y88" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP88" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ88" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW88" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC88" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF88" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG88" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH88" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI88" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="B89" s="4">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="C89">
+        <v>6</v>
+      </c>
+      <c r="D89" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>49</v>
+      </c>
+      <c r="F89" t="s">
+        <v>49</v>
+      </c>
+      <c r="G89" t="s">
+        <v>3</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P89" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>49</v>
+      </c>
+      <c r="R89" t="s">
+        <v>49</v>
+      </c>
+      <c r="S89" t="s">
+        <v>1</v>
+      </c>
+      <c r="V89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP89" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV89" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG89" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH89" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A90" s="4">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="B90" s="4">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="C90">
+        <v>9</v>
+      </c>
+      <c r="D90" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>1</v>
+      </c>
+      <c r="F90" t="s">
+        <v>49</v>
+      </c>
+      <c r="G90" t="s">
+        <v>1</v>
+      </c>
+      <c r="J90" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K90" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L90" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M90" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P90" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>49</v>
+      </c>
+      <c r="R90" t="s">
+        <v>49</v>
+      </c>
+      <c r="S90" t="s">
+        <v>1</v>
+      </c>
+      <c r="V90" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W90" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X90" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y90" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP90" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ90" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU90" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV90" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW90" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA90" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB90" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF90" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BG90" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH90" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="B91" s="4">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="C91">
+        <v>13</v>
+      </c>
+      <c r="D91" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G91" t="s">
+        <v>5</v>
+      </c>
+      <c r="J91" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K91" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L91" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M91" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P91" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>1</v>
+      </c>
+      <c r="R91" t="s">
+        <v>1</v>
+      </c>
+      <c r="S91" t="s">
+        <v>5</v>
+      </c>
+      <c r="V91" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W91" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X91" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y91" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP91" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ91" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT91" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU91" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW91" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ91" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC91" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF91" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG91" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH91" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI91" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B92" s="4">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="C92">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" t="s">
+        <v>3</v>
+      </c>
+      <c r="F92" t="s">
+        <v>49</v>
+      </c>
+      <c r="G92" t="s">
+        <v>49</v>
+      </c>
+      <c r="J92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P92" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>49</v>
+      </c>
+      <c r="R92" t="s">
+        <v>49</v>
+      </c>
+      <c r="S92" t="s">
+        <v>49</v>
+      </c>
+      <c r="V92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP92" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV92" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW92" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA92" t="s">
+        <v>45</v>
+      </c>
+      <c r="BC92" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF92" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG92" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI92" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="93" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="B93" s="4">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="C93">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1</v>
+      </c>
+      <c r="G93" t="s">
+        <v>1</v>
+      </c>
+      <c r="J93" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K93" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L93" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M93" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P93" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>49</v>
+      </c>
+      <c r="R93" t="s">
+        <v>49</v>
+      </c>
+      <c r="S93" t="s">
+        <v>49</v>
+      </c>
+      <c r="V93" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W93" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X93" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y93" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO93" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP93" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ93" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW93" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ93" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA93" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB93" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF93" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH93" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A94" s="4">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="B94" s="4">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="C94">
+        <v>7</v>
+      </c>
+      <c r="D94" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>49</v>
+      </c>
+      <c r="F94" t="s">
+        <v>49</v>
+      </c>
+      <c r="G94" t="s">
+        <v>1</v>
+      </c>
+      <c r="J94" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K94" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L94" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M94" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P94" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>49</v>
+      </c>
+      <c r="R94" t="s">
+        <v>1</v>
+      </c>
+      <c r="S94" t="s">
+        <v>1</v>
+      </c>
+      <c r="V94" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W94" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X94" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y94" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO94" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ94" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV94" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW94" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ94" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB94" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC94" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI94" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="B95" s="4">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="C95">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>3</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1</v>
+      </c>
+      <c r="G95" t="s">
+        <v>1</v>
+      </c>
+      <c r="J95" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L95" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M95" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P95" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>49</v>
+      </c>
+      <c r="R95" t="s">
+        <v>49</v>
+      </c>
+      <c r="S95" t="s">
+        <v>1</v>
+      </c>
+      <c r="V95" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W95" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X95" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y95" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP95" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU95" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW95" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA95" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC95" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG95" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH95" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI95" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="B96" s="4">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="C96">
+        <v>10</v>
+      </c>
+      <c r="D96" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" t="s">
+        <v>1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1</v>
+      </c>
+      <c r="G96" t="s">
+        <v>1</v>
+      </c>
+      <c r="J96" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K96" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L96" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M96" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P96" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>49</v>
+      </c>
+      <c r="R96" t="s">
+        <v>49</v>
+      </c>
+      <c r="S96" t="s">
+        <v>1</v>
+      </c>
+      <c r="V96" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W96" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X96" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y96" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ96" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW96" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB96" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC96" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF96" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG96" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BH96" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="B97" s="4">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="C97">
+        <v>9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1</v>
+      </c>
+      <c r="G97" t="s">
+        <v>3</v>
+      </c>
+      <c r="J97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P97" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>49</v>
+      </c>
+      <c r="R97" t="s">
+        <v>49</v>
+      </c>
+      <c r="S97" t="s">
+        <v>49</v>
+      </c>
+      <c r="V97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV97" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW97" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB97" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC97" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF97" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG97" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="BH97" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BI97" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A98" s="4">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="B98" s="4">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="C98">
+        <v>7</v>
+      </c>
+      <c r="D98" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>49</v>
+      </c>
+      <c r="F98" t="s">
+        <v>49</v>
+      </c>
+      <c r="G98" t="s">
+        <v>5</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L98" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M98" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P98" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>5</v>
+      </c>
+      <c r="R98" t="s">
+        <v>5</v>
+      </c>
+      <c r="S98" t="s">
+        <v>49</v>
+      </c>
+      <c r="V98" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W98" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X98" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y98" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ98" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT98" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW98" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ98" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC98" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF98" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG98" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="99" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A99" s="4">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="B99" s="4">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="C99">
+        <v>11</v>
+      </c>
+      <c r="D99" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>49</v>
+      </c>
+      <c r="F99" t="s">
+        <v>5</v>
+      </c>
+      <c r="G99" t="s">
+        <v>49</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K99" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L99" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M99" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P99" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>49</v>
+      </c>
+      <c r="R99" t="s">
+        <v>5</v>
+      </c>
+      <c r="S99" t="s">
+        <v>49</v>
+      </c>
+      <c r="V99" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W99" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X99" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y99" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO99" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV99" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW99" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA99" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG99" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI99" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A100" s="4">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="B100" s="4">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="C100">
+        <v>15</v>
+      </c>
+      <c r="D100" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" t="s">
+        <v>5</v>
+      </c>
+      <c r="F100" t="s">
+        <v>49</v>
+      </c>
+      <c r="G100" t="s">
+        <v>5</v>
+      </c>
+      <c r="J100" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L100" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M100" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P100" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>49</v>
+      </c>
+      <c r="R100" t="s">
+        <v>49</v>
+      </c>
+      <c r="S100" t="s">
+        <v>49</v>
+      </c>
+      <c r="V100" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W100" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X100" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y100" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO100" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP100" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT100" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU100" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB100" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC100" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG100" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH100" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A101" s="4">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="B101" s="4">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+      <c r="C101">
+        <v>11</v>
+      </c>
+      <c r="D101" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" t="s">
+        <v>3</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1</v>
+      </c>
+      <c r="G101" t="s">
+        <v>1</v>
+      </c>
+      <c r="J101" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K101" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L101" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M101" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P101" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>49</v>
+      </c>
+      <c r="R101" t="s">
+        <v>49</v>
+      </c>
+      <c r="S101" t="s">
+        <v>5</v>
+      </c>
+      <c r="V101" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W101" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="X101" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y101" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ101" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW101" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ101" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH101" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BI101" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A102" s="4">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B102" s="4">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="C102">
+        <v>14</v>
+      </c>
+      <c r="D102" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" t="s">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1</v>
+      </c>
+      <c r="G102" t="s">
+        <v>1</v>
+      </c>
+      <c r="H102" t="s">
+        <v>1</v>
+      </c>
+      <c r="J102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P102" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>1</v>
+      </c>
+      <c r="R102" t="s">
+        <v>1</v>
+      </c>
+      <c r="S102" t="s">
+        <v>1</v>
+      </c>
+      <c r="T102" t="s">
+        <v>1</v>
+      </c>
+      <c r="V102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z102" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB102" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC102" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD102" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE102" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF102" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO102" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP102" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ102" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR102" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT102" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU102" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV102" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW102" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX102" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ102" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA102" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB102" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC102" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD102" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF102" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG102" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH102" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI102" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ102" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL102" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM102" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN102" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A103" s="4">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="B103" s="4">
+        <f t="shared" si="3"/>
+        <v>101</v>
+      </c>
+      <c r="C103">
+        <v>19</v>
+      </c>
+      <c r="D103" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" t="s">
+        <v>1</v>
+      </c>
+      <c r="F103" t="s">
+        <v>5</v>
+      </c>
+      <c r="G103" t="s">
+        <v>5</v>
+      </c>
+      <c r="H103" t="s">
+        <v>5</v>
+      </c>
+      <c r="J103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K103" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M103" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P103" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>1</v>
+      </c>
+      <c r="R103" t="s">
+        <v>3</v>
+      </c>
+      <c r="S103" t="s">
+        <v>1</v>
+      </c>
+      <c r="T103" t="s">
+        <v>49</v>
+      </c>
+      <c r="V103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W103" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X103" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y103" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB103" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC103" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD103" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE103" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF103" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO103" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT103" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU103" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW103" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX103" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ103" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA103" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC103" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG103" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH103" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI103" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BJ103" s="8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>